<commit_message>
added dynamic asset pricing, changed file structure
</commit_message>
<xml_diff>
--- a/run.xlsx
+++ b/run.xlsx
@@ -433,7 +433,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>number_of_traders</t>
+          <t>oi_short</t>
         </is>
       </c>
     </row>
@@ -443,7 +443,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>number_of_liquidations</t>
+          <t>pool_balance_btc</t>
         </is>
       </c>
     </row>
@@ -463,7 +463,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>volume_sol</t>
+          <t>volume_eth</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>volume_btc</t>
+          <t>number_of_liquidations</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>treasury_balance</t>
+          <t>volume_sol</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>pool_balance_usdT</t>
+          <t>treasury_balance</t>
         </is>
       </c>
     </row>
@@ -503,7 +503,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>pool_balance_sol</t>
+          <t>pool_balance_usdc</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>oi_long</t>
+          <t>min_pnl_traders</t>
         </is>
       </c>
     </row>
@@ -523,7 +523,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>pool_balance_usdc</t>
+          <t>number_of_traders</t>
         </is>
       </c>
     </row>
@@ -533,7 +533,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>fees_collected</t>
+          <t>pool_balance_usdT</t>
         </is>
       </c>
     </row>
@@ -543,7 +543,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>number_of_liquidity_providers</t>
+          <t>fees_collected</t>
         </is>
       </c>
     </row>
@@ -553,7 +553,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>max_pnl_traders</t>
+          <t>cum_pnl_traders</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>cum_pnl_traders</t>
+          <t>volume_btc</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>min_pnl_traders</t>
+          <t>pool_balance_eth</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>pool_balance_eth</t>
+          <t>oi_long</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>volume_eth</t>
+          <t>pool_balance_sol</t>
         </is>
       </c>
     </row>
@@ -603,7 +603,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>pool_balance_btc</t>
+          <t>max_pnl_traders</t>
         </is>
       </c>
     </row>
@@ -613,7 +613,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>oi_short</t>
+          <t>number_of_liquidity_providers</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
minor bug fixes, swaps added
</commit_message>
<xml_diff>
--- a/run.xlsx
+++ b/run.xlsx
@@ -433,7 +433,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>oi_short</t>
+          <t>pool_balance_sol</t>
         </is>
       </c>
     </row>
@@ -443,7 +443,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>pool_balance_btc</t>
+          <t>number_of_liquidations</t>
         </is>
       </c>
     </row>
@@ -453,7 +453,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>cum_apy_providers</t>
+          <t>volume_eth</t>
         </is>
       </c>
     </row>
@@ -463,7 +463,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>volume_eth</t>
+          <t>treasury_balance</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>number_of_liquidations</t>
+          <t>oi_short</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>volume_sol</t>
+          <t>pool_balance_usdT</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>treasury_balance</t>
+          <t>cum_apy_providers</t>
         </is>
       </c>
     </row>
@@ -503,7 +503,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>pool_balance_usdc</t>
+          <t>oi_long</t>
         </is>
       </c>
     </row>
@@ -523,7 +523,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>number_of_traders</t>
+          <t>fees_collected</t>
         </is>
       </c>
     </row>
@@ -533,7 +533,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>pool_balance_usdT</t>
+          <t>pool_balance_btc</t>
         </is>
       </c>
     </row>
@@ -543,7 +543,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>fees_collected</t>
+          <t>pool_balance_eth</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>volume_btc</t>
+          <t>number_of_traders</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>pool_balance_eth</t>
+          <t>volume_sol</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>oi_long</t>
+          <t>volume_btc</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>pool_balance_sol</t>
+          <t>max_pnl_traders</t>
         </is>
       </c>
     </row>
@@ -603,7 +603,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>max_pnl_traders</t>
+          <t>number_of_liquidity_providers</t>
         </is>
       </c>
     </row>
@@ -613,7 +613,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>number_of_liquidity_providers</t>
+          <t>pool_balance_usdc</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed issue with shorts
</commit_message>
<xml_diff>
--- a/run.xlsx
+++ b/run.xlsx
@@ -819,19 +819,19 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>10.01003949404379</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
         <v>110</v>
       </c>
       <c r="F5" t="n">
-        <v>2497.340245797123</v>
+        <v>2500</v>
       </c>
       <c r="G5" t="n">
-        <v>451356.565507693</v>
+        <v>450000</v>
       </c>
       <c r="H5" t="n">
-        <v>448645.3738817211</v>
+        <v>450000</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -846,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -864,37 +864,37 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="T5" t="n">
         <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
         <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>0.03084603303462075</v>
+        <v>0.008161764201742479</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.001558687734908661</v>
+        <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
+        <v>0.002448529260522744</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.004635017637930755</v>
+        <v>0</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.00152999776331258</v>
+        <v>0</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.00153010677423423</v>
+        <v>0</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
@@ -909,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="AH5" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="AI5" t="n">
         <v>0</v>
@@ -926,19 +926,19 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>10.01003949404379</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
         <v>110</v>
       </c>
       <c r="F6" t="n">
-        <v>2497.340245797123</v>
+        <v>2500</v>
       </c>
       <c r="G6" t="n">
-        <v>451356.565507693</v>
+        <v>450000</v>
       </c>
       <c r="H6" t="n">
-        <v>448645.3738817211</v>
+        <v>450000</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -971,37 +971,37 @@
         <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W6" t="n">
         <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>0.03084603303462075</v>
+        <v>0.008161764201742479</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.001558687734908661</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>0</v>
+        <v>0.002448529260522744</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.004635017637930755</v>
+        <v>0</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.00152999776331258</v>
+        <v>0</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.00153010677423423</v>
+        <v>0</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -1016,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="AH6" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="AI6" t="n">
         <v>0</v>
@@ -1033,19 +1033,19 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>9.973093468114753</v>
+        <v>9.952012308474941</v>
       </c>
       <c r="E7" t="n">
-        <v>109.344429027126</v>
+        <v>110</v>
       </c>
       <c r="F7" t="n">
-        <v>2493.863248885385</v>
+        <v>2507.221595856023</v>
       </c>
       <c r="G7" t="n">
-        <v>451356.565507693</v>
+        <v>451126.8423264105</v>
       </c>
       <c r="H7" t="n">
-        <v>453466.3481028817</v>
+        <v>449845.8003643745</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
@@ -1072,43 +1072,43 @@
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>4.716014480118543</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="T7" t="n">
-        <v>0</v>
+        <v>4.716014480118543</v>
       </c>
       <c r="U7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V7" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="W7" t="n">
         <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>0.0722875420339829</v>
+        <v>0.03918773730027794</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.006293277141840933</v>
+        <v>0.003171883362531667</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.00156154030457871</v>
+        <v>0.002448529260522744</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.006179752624097776</v>
+        <v>0.001546299491078141</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.004591585701158199</v>
+        <v>0.003059156421594817</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.00306010683851925</v>
+        <v>0.001530452654356013</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -1123,10 +1123,10 @@
         <v>0</v>
       </c>
       <c r="AH7" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="AI7" t="n">
-        <v>0</v>
+        <v>-4.716014480118543</v>
       </c>
     </row>
     <row r="8">
@@ -1140,19 +1140,19 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>9.973093468114753</v>
+        <v>9.952012308474941</v>
       </c>
       <c r="E8" t="n">
-        <v>109.344429027126</v>
+        <v>110</v>
       </c>
       <c r="F8" t="n">
-        <v>2493.863248885385</v>
+        <v>2507.221595856023</v>
       </c>
       <c r="G8" t="n">
-        <v>451356.565507693</v>
+        <v>451126.8423264105</v>
       </c>
       <c r="H8" t="n">
-        <v>453466.3481028817</v>
+        <v>449845.8003643745</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
@@ -1179,43 +1179,43 @@
         <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>4.716014480118543</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="T8" t="n">
-        <v>0</v>
+        <v>4.716014480118543</v>
       </c>
       <c r="U8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V8" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="W8" t="n">
         <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>0.0722875420339829</v>
+        <v>0.03918773730027794</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.006293277141840933</v>
+        <v>0.003171883362531667</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.00156154030457871</v>
+        <v>0.002448529260522744</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.006179752624097776</v>
+        <v>0.001546299491078141</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.004591585701158199</v>
+        <v>0.003059156421594817</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.00306010683851925</v>
+        <v>0.001530452654356013</v>
       </c>
       <c r="AD8" t="n">
         <v>0</v>
@@ -1230,10 +1230,10 @@
         <v>0</v>
       </c>
       <c r="AH8" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="AI8" t="n">
-        <v>0</v>
+        <v>-4.716014480118543</v>
       </c>
     </row>
     <row r="9">
@@ -1247,19 +1247,19 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>9.970471150932532</v>
+        <v>9.927592572308125</v>
       </c>
       <c r="E9" t="n">
-        <v>109.524437738273</v>
+        <v>110.2938377365662</v>
       </c>
       <c r="F9" t="n">
-        <v>2487.570835224308</v>
+        <v>2507.221595856023</v>
       </c>
       <c r="G9" t="n">
-        <v>451862.7953467346</v>
+        <v>451126.8423264105</v>
       </c>
       <c r="H9" t="n">
-        <v>453466.3481028817</v>
+        <v>449845.8003643745</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -1271,10 +1271,10 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.3520423332118753</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="N9" t="n">
         <v>0</v>
@@ -1283,46 +1283,46 @@
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>0.03797181152499512</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>23.36555975972203</v>
       </c>
       <c r="R9" t="n">
-        <v>0.3520423332118753</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>0</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T9" t="n">
-        <v>0</v>
+        <v>23.36555975972203</v>
       </c>
       <c r="U9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V9" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="W9" t="n">
         <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>0.1072228317855425</v>
+        <v>0.04974599627813001</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.008948419918762628</v>
+        <v>0.004754654151732103</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.006321539595842425</v>
+        <v>0.004033236164677929</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.007716191455963528</v>
+        <v>0.001546299491078141</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.006120591726574916</v>
+        <v>0.003059156421594817</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.00306010683851925</v>
+        <v>0.001530452654356013</v>
       </c>
       <c r="AD9" t="n">
         <v>0</v>
@@ -1334,13 +1334,13 @@
         <v>0</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.3520423332118753</v>
+        <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>0</v>
+        <v>0.7478821251388056</v>
       </c>
       <c r="AI9" t="n">
-        <v>0</v>
+        <v>-23.36555975972203</v>
       </c>
     </row>
     <row r="10">
@@ -1354,19 +1354,19 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>9.970471150932532</v>
+        <v>9.927592572308125</v>
       </c>
       <c r="E10" t="n">
-        <v>109.524437738273</v>
+        <v>110.2938377365662</v>
       </c>
       <c r="F10" t="n">
-        <v>2487.570835224308</v>
+        <v>2507.221595856023</v>
       </c>
       <c r="G10" t="n">
-        <v>451862.7953467346</v>
+        <v>451126.8423264105</v>
       </c>
       <c r="H10" t="n">
-        <v>453466.3481028817</v>
+        <v>449845.8003643745</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -1378,10 +1378,10 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0.3520423332118753</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
@@ -1390,46 +1390,46 @@
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>0.03797181152499512</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>23.36555975972203</v>
       </c>
       <c r="R10" t="n">
-        <v>0.3520423332118753</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T10" t="n">
-        <v>0</v>
+        <v>23.36555975972203</v>
       </c>
       <c r="U10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V10" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="W10" t="n">
         <v>0</v>
       </c>
       <c r="X10" t="n">
-        <v>0.1072228317855425</v>
+        <v>0.04974599627813001</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.008948419918762628</v>
+        <v>0.004754654151732103</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.006321539595842425</v>
+        <v>0.004033236164677929</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.007716191455963528</v>
+        <v>0.001546299491078141</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.006120591726574916</v>
+        <v>0.003059156421594817</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.00306010683851925</v>
+        <v>0.001530452654356013</v>
       </c>
       <c r="AD10" t="n">
         <v>0</v>
@@ -1441,13 +1441,13 @@
         <v>0</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.3520423332118753</v>
+        <v>0</v>
       </c>
       <c r="AH10" t="n">
-        <v>0</v>
+        <v>0.7478821251388056</v>
       </c>
       <c r="AI10" t="n">
-        <v>0</v>
+        <v>-23.36555975972203</v>
       </c>
     </row>
     <row r="11">
@@ -1461,82 +1461,82 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>10.04459076654763</v>
+        <v>9.927592572308125</v>
       </c>
       <c r="E11" t="n">
-        <v>111.2779433733329</v>
+        <v>110.2938377365662</v>
       </c>
       <c r="F11" t="n">
-        <v>2487.570835224308</v>
+        <v>2507.221595856023</v>
       </c>
       <c r="G11" t="n">
-        <v>448494.7474570213</v>
+        <v>451134.8114145231</v>
       </c>
       <c r="H11" t="n">
-        <v>447503.3841271785</v>
+        <v>449837.8286230432</v>
       </c>
       <c r="I11" t="n">
-        <v>-440.0354272447158</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>-440.0354272447158</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>-440.0354272447158</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>0.03797181152499512</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R11" t="n">
-        <v>0.3520423332118753</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="S11" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T11" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="V11" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="W11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X11" t="n">
-        <v>0.1534914613219356</v>
+        <v>0.0599401107625509</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.0131548524831716</v>
+        <v>0.004754654151732103</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.01136507516103109</v>
+        <v>0.004033236164677929</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.007716191455963528</v>
+        <v>0.001546299491078141</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.00766284852832657</v>
+        <v>0.004580477483712365</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.006148470768087898</v>
+        <v>0.003067365937564734</v>
       </c>
       <c r="AD11" t="n">
         <v>0</v>
@@ -1548,13 +1548,13 @@
         <v>0</v>
       </c>
       <c r="AG11" t="n">
-        <v>0</v>
+        <v>-0.007400726221988298</v>
       </c>
       <c r="AH11" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.7478821251388056</v>
       </c>
       <c r="AI11" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="12">
@@ -1568,82 +1568,82 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>10.04459076654763</v>
+        <v>9.927592572308125</v>
       </c>
       <c r="E12" t="n">
-        <v>111.2779433733329</v>
+        <v>110.2938377365662</v>
       </c>
       <c r="F12" t="n">
-        <v>2487.570835224308</v>
+        <v>2507.221595856023</v>
       </c>
       <c r="G12" t="n">
-        <v>448494.7474570213</v>
+        <v>451134.8114145231</v>
       </c>
       <c r="H12" t="n">
-        <v>447503.3841271785</v>
+        <v>449837.8286230432</v>
       </c>
       <c r="I12" t="n">
-        <v>-440.0354272447158</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>-440.0354272447158</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>-440.0354272447158</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>0.03797181152499512</v>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R12" t="n">
-        <v>0.3520423332118753</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="S12" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T12" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U12" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="V12" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="W12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X12" t="n">
-        <v>0.1534914613219356</v>
+        <v>0.0599401107625509</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.0131548524831716</v>
+        <v>0.004754654151732103</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.01136507516103109</v>
+        <v>0.004033236164677929</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.007716191455963528</v>
+        <v>0.001546299491078141</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.00766284852832657</v>
+        <v>0.004580477483712365</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.006148470768087898</v>
+        <v>0.003067365937564734</v>
       </c>
       <c r="AD12" t="n">
         <v>0</v>
@@ -1655,13 +1655,13 @@
         <v>0</v>
       </c>
       <c r="AG12" t="n">
-        <v>0</v>
+        <v>-0.007400726221988298</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.7478821251388056</v>
       </c>
       <c r="AI12" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="13">
@@ -1675,82 +1675,82 @@
         <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>10.04459076654763</v>
+        <v>9.923021202883046</v>
       </c>
       <c r="E13" t="n">
-        <v>111.2772185745058</v>
+        <v>110.3498261031847</v>
       </c>
       <c r="F13" t="n">
-        <v>2487.570835224308</v>
+        <v>2507.221595856023</v>
       </c>
       <c r="G13" t="n">
-        <v>448494.7474570213</v>
+        <v>451134.8114145231</v>
       </c>
       <c r="H13" t="n">
-        <v>447503.3841271785</v>
+        <v>449837.8286230432</v>
       </c>
       <c r="I13" t="n">
-        <v>-437.471099866318</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>-437.471099866318</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>-437.471099866318</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>0.03797181152499512</v>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R13" t="n">
-        <v>0.3520423332118753</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="S13" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T13" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U13" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="V13" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="W13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X13" t="n">
-        <v>0.1646622945103897</v>
+        <v>0.0705702789282852</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.0131548524831716</v>
+        <v>0.006330745892397074</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.01162078508761589</v>
+        <v>0.005646194873733246</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.01081173148591496</v>
+        <v>0.001546299491078141</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.00766284852832657</v>
+        <v>0.004580477483712365</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.006148470768087898</v>
+        <v>0.003067365937564734</v>
       </c>
       <c r="AD13" t="n">
         <v>0</v>
@@ -1762,13 +1762,13 @@
         <v>0</v>
       </c>
       <c r="AG13" t="n">
-        <v>0</v>
+        <v>-0.007400726221988298</v>
       </c>
       <c r="AH13" t="n">
-        <v>0</v>
+        <v>0.7478821251388056</v>
       </c>
       <c r="AI13" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="14">
@@ -1782,82 +1782,82 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>10.04459076654763</v>
+        <v>9.923021202883046</v>
       </c>
       <c r="E14" t="n">
-        <v>111.2772185745058</v>
+        <v>110.3498261031847</v>
       </c>
       <c r="F14" t="n">
-        <v>2487.570835224308</v>
+        <v>2507.221595856023</v>
       </c>
       <c r="G14" t="n">
-        <v>448494.7474570213</v>
+        <v>451134.8114145231</v>
       </c>
       <c r="H14" t="n">
-        <v>447503.3841271785</v>
+        <v>449837.8286230432</v>
       </c>
       <c r="I14" t="n">
-        <v>-437.471099866318</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>-437.471099866318</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>-437.471099866318</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
         <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>0.7858539366638007</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>0.03797181152499512</v>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R14" t="n">
-        <v>0.3520423332118753</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="S14" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T14" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U14" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="V14" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="W14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X14" t="n">
-        <v>0.1646622945103897</v>
+        <v>0.0705702789282852</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.0131548524831716</v>
+        <v>0.006330745892397074</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.01162078508761589</v>
+        <v>0.005646194873733246</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.01081173148591496</v>
+        <v>0.001546299491078141</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.00766284852832657</v>
+        <v>0.004580477483712365</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.006148470768087898</v>
+        <v>0.003067365937564734</v>
       </c>
       <c r="AD14" t="n">
         <v>0</v>
@@ -1869,13 +1869,13 @@
         <v>0</v>
       </c>
       <c r="AG14" t="n">
-        <v>0</v>
+        <v>-0.007400726221988298</v>
       </c>
       <c r="AH14" t="n">
-        <v>0</v>
+        <v>0.7478821251388056</v>
       </c>
       <c r="AI14" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="15">
@@ -1889,28 +1889,28 @@
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>10.04459076654763</v>
+        <v>9.923804706719947</v>
       </c>
       <c r="E15" t="n">
-        <v>111.2772185745058</v>
+        <v>109.6954693175245</v>
       </c>
       <c r="F15" t="n">
-        <v>2487.570835224308</v>
+        <v>2524.743633547097</v>
       </c>
       <c r="G15" t="n">
-        <v>448494.7474570213</v>
+        <v>451134.8114145231</v>
       </c>
       <c r="H15" t="n">
-        <v>447503.3841271785</v>
+        <v>449804.923651695</v>
       </c>
       <c r="I15" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="J15" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="K15" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="L15" t="n">
         <v>0</v>
@@ -1922,49 +1922,49 @@
         <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="P15" t="n">
-        <v>0</v>
+        <v>0.03797181152499512</v>
       </c>
       <c r="Q15" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R15" t="n">
-        <v>0.3520423332118753</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="S15" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T15" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U15" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V15" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="W15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X15" t="n">
-        <v>0.1749378204931825</v>
+        <v>0.09965899571287148</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.0131548524831716</v>
+        <v>0.00790196168402147</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.01162078508761589</v>
+        <v>0.009339395665117078</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.01081173148591496</v>
+        <v>0.003327373817330791</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.00766284852832657</v>
+        <v>0.004580477483712365</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.009231128562925729</v>
+        <v>0.004748490063679736</v>
       </c>
       <c r="AD15" t="n">
         <v>0</v>
@@ -1976,13 +1976,13 @@
         <v>0</v>
       </c>
       <c r="AG15" t="n">
-        <v>0</v>
+        <v>-0.007400726221988298</v>
       </c>
       <c r="AH15" t="n">
-        <v>0</v>
+        <v>-0.03797181152499512</v>
       </c>
       <c r="AI15" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="16">
@@ -1996,28 +1996,28 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>10.04459076654763</v>
+        <v>9.923804706719947</v>
       </c>
       <c r="E16" t="n">
-        <v>111.2772185745058</v>
+        <v>109.6954693175245</v>
       </c>
       <c r="F16" t="n">
-        <v>2487.570835224308</v>
+        <v>2524.743633547097</v>
       </c>
       <c r="G16" t="n">
-        <v>448494.7474570213</v>
+        <v>451134.8114145231</v>
       </c>
       <c r="H16" t="n">
-        <v>447503.3841271785</v>
+        <v>449804.923651695</v>
       </c>
       <c r="I16" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="J16" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="K16" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
@@ -2029,49 +2029,49 @@
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="P16" t="n">
-        <v>0</v>
+        <v>0.03797181152499512</v>
       </c>
       <c r="Q16" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R16" t="n">
-        <v>0.3520423332118753</v>
+        <v>0.007400726221988298</v>
       </c>
       <c r="S16" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T16" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U16" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V16" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="W16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X16" t="n">
-        <v>0.1749378204931825</v>
+        <v>0.09965899571287148</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.0131548524831716</v>
+        <v>0.00790196168402147</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.01162078508761589</v>
+        <v>0.009339395665117078</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.01081173148591496</v>
+        <v>0.003327373817330791</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.00766284852832657</v>
+        <v>0.004580477483712365</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.009231128562925729</v>
+        <v>0.004748490063679736</v>
       </c>
       <c r="AD16" t="n">
         <v>0</v>
@@ -2083,13 +2083,13 @@
         <v>0</v>
       </c>
       <c r="AG16" t="n">
-        <v>0</v>
+        <v>-0.007400726221988298</v>
       </c>
       <c r="AH16" t="n">
-        <v>0</v>
+        <v>-0.03797181152499512</v>
       </c>
       <c r="AI16" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="17">
@@ -2103,28 +2103,28 @@
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>10.04459076654763</v>
+        <v>9.923804706719947</v>
       </c>
       <c r="E17" t="n">
-        <v>111.2772185745058</v>
+        <v>109.2148018306021</v>
       </c>
       <c r="F17" t="n">
-        <v>2487.570835224308</v>
+        <v>2524.743633547097</v>
       </c>
       <c r="G17" t="n">
-        <v>448494.7474570213</v>
+        <v>452626.9081982066</v>
       </c>
       <c r="H17" t="n">
-        <v>447503.3841271785</v>
+        <v>449804.923651695</v>
       </c>
       <c r="I17" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="J17" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="K17" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
@@ -2136,67 +2136,67 @@
         <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>0.008905804457888288</v>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
+        <v>0.03797181152499512</v>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R17" t="n">
-        <v>0.3520423332118753</v>
+        <v>0.008905804457888288</v>
       </c>
       <c r="S17" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T17" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U17" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="V17" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="W17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X17" t="n">
-        <v>0.1851919326879622</v>
+        <v>0.1083945960163406</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.0131548524831716</v>
+        <v>0.00790196168402147</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.01162078508761589</v>
+        <v>0.01057084028497358</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.01081173148591496</v>
+        <v>0.003327373817330791</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.00766284852832657</v>
+        <v>0.005969712954896607</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.01230736222135963</v>
+        <v>0.004748490063679736</v>
       </c>
       <c r="AD17" t="n">
         <v>0</v>
       </c>
       <c r="AE17" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF17" t="n">
         <v>0</v>
       </c>
       <c r="AG17" t="n">
-        <v>0</v>
+        <v>-0.008905804457888288</v>
       </c>
       <c r="AH17" t="n">
-        <v>0</v>
+        <v>-0.03797181152499512</v>
       </c>
       <c r="AI17" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="18">
@@ -2210,28 +2210,28 @@
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>10.04459076654763</v>
+        <v>9.923804706719947</v>
       </c>
       <c r="E18" t="n">
-        <v>111.2772185745058</v>
+        <v>109.2148018306021</v>
       </c>
       <c r="F18" t="n">
-        <v>2487.570835224308</v>
+        <v>2524.743633547097</v>
       </c>
       <c r="G18" t="n">
-        <v>448494.7474570213</v>
+        <v>452626.9081982066</v>
       </c>
       <c r="H18" t="n">
-        <v>447503.3841271785</v>
+        <v>449804.923651695</v>
       </c>
       <c r="I18" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="J18" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="K18" t="n">
-        <v>-437.471099866318</v>
+        <v>-424.0557340696678</v>
       </c>
       <c r="L18" t="n">
         <v>0</v>
@@ -2243,67 +2243,67 @@
         <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>0</v>
+        <v>0.008905804457888288</v>
       </c>
       <c r="P18" t="n">
-        <v>0</v>
+        <v>0.03797181152499512</v>
       </c>
       <c r="Q18" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R18" t="n">
-        <v>0.3520423332118753</v>
+        <v>0.008905804457888288</v>
       </c>
       <c r="S18" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T18" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U18" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="V18" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="W18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X18" t="n">
-        <v>0.1851919326879622</v>
+        <v>0.1083945960163406</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.0131548524831716</v>
+        <v>0.00790196168402147</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.01162078508761589</v>
+        <v>0.01057084028497358</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.01081173148591496</v>
+        <v>0.003327373817330791</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.00766284852832657</v>
+        <v>0.005969712954896607</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.01230736222135963</v>
+        <v>0.004748490063679736</v>
       </c>
       <c r="AD18" t="n">
         <v>0</v>
       </c>
       <c r="AE18" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF18" t="n">
         <v>0</v>
       </c>
       <c r="AG18" t="n">
-        <v>0</v>
+        <v>-0.008905804457888288</v>
       </c>
       <c r="AH18" t="n">
-        <v>0</v>
+        <v>-0.03797181152499512</v>
       </c>
       <c r="AI18" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="19">
@@ -2317,28 +2317,28 @@
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>9.934514359651642</v>
+        <v>9.932803303958034</v>
       </c>
       <c r="E19" t="n">
-        <v>111.2772185745058</v>
+        <v>109.2148018306021</v>
       </c>
       <c r="F19" t="n">
-        <v>2487.570835224308</v>
+        <v>2524.743633547097</v>
       </c>
       <c r="G19" t="n">
-        <v>453167.3359840115</v>
+        <v>452223.09562382</v>
       </c>
       <c r="H19" t="n">
-        <v>447503.3841271785</v>
+        <v>449804.923651695</v>
       </c>
       <c r="I19" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="J19" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="K19" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="L19" t="n">
         <v>0</v>
@@ -2350,67 +2350,67 @@
         <v>0</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>0.1081128836816244</v>
       </c>
       <c r="P19" t="n">
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R19" t="n">
-        <v>0.3520423332118753</v>
+        <v>0.1081128836816244</v>
       </c>
       <c r="S19" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T19" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U19" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="V19" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="W19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X19" t="n">
-        <v>0.1953471006931808</v>
+        <v>0.1197175256811012</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.01475497173550951</v>
+        <v>0.009475358629791238</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.01162078508761589</v>
+        <v>0.01057084028497358</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.01081173148591496</v>
+        <v>0.003327373817330791</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.009109279677554262</v>
+        <v>0.007793194908555012</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.01230736222135963</v>
+        <v>0.004748490063679736</v>
       </c>
       <c r="AD19" t="n">
         <v>0</v>
       </c>
       <c r="AE19" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF19" t="n">
         <v>0</v>
       </c>
       <c r="AG19" t="n">
-        <v>0</v>
+        <v>-0.1081128836816244</v>
       </c>
       <c r="AH19" t="n">
         <v>0</v>
       </c>
       <c r="AI19" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="20">
@@ -2424,28 +2424,28 @@
         <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>9.934514359651642</v>
+        <v>9.932803303958034</v>
       </c>
       <c r="E20" t="n">
-        <v>111.2772185745058</v>
+        <v>109.2148018306021</v>
       </c>
       <c r="F20" t="n">
-        <v>2487.570835224308</v>
+        <v>2524.743633547097</v>
       </c>
       <c r="G20" t="n">
-        <v>453167.3359840115</v>
+        <v>452223.09562382</v>
       </c>
       <c r="H20" t="n">
-        <v>447503.3841271785</v>
+        <v>449804.923651695</v>
       </c>
       <c r="I20" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="J20" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="K20" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="L20" t="n">
         <v>0</v>
@@ -2457,67 +2457,67 @@
         <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>0</v>
+        <v>0.1081128836816244</v>
       </c>
       <c r="P20" t="n">
         <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R20" t="n">
-        <v>0.3520423332118753</v>
+        <v>0.1081128836816244</v>
       </c>
       <c r="S20" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.8238257481887957</v>
       </c>
       <c r="T20" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U20" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="V20" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="W20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X20" t="n">
-        <v>0.1953471006931808</v>
+        <v>0.1197175256811012</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.01475497173550951</v>
+        <v>0.009475358629791238</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.01162078508761589</v>
+        <v>0.01057084028497358</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.01081173148591496</v>
+        <v>0.003327373817330791</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.009109279677554262</v>
+        <v>0.007793194908555012</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.01230736222135963</v>
+        <v>0.004748490063679736</v>
       </c>
       <c r="AD20" t="n">
         <v>0</v>
       </c>
       <c r="AE20" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF20" t="n">
         <v>0</v>
       </c>
       <c r="AG20" t="n">
-        <v>0</v>
+        <v>-0.1081128836816244</v>
       </c>
       <c r="AH20" t="n">
         <v>0</v>
       </c>
       <c r="AI20" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="21">
@@ -2531,100 +2531,100 @@
         <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>9.941107077606285</v>
+        <v>9.932596085307081</v>
       </c>
       <c r="E21" t="n">
-        <v>111.184889376806</v>
+        <v>109.2175520736144</v>
       </c>
       <c r="F21" t="n">
-        <v>2487.570835224308</v>
+        <v>2541.59792883567</v>
       </c>
       <c r="G21" t="n">
-        <v>453167.3359840115</v>
+        <v>449938.2170230591</v>
       </c>
       <c r="H21" t="n">
-        <v>447503.3841271785</v>
+        <v>449798.1704235579</v>
       </c>
       <c r="I21" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="J21" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="K21" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="L21" t="n">
-        <v>0.001314990729519657</v>
+        <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N21" t="n">
         <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>0</v>
+        <v>0.2022937416699535</v>
       </c>
       <c r="P21" t="n">
         <v>0</v>
       </c>
       <c r="Q21" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R21" t="n">
-        <v>0.353357323941395</v>
+        <v>0.2022937416699535</v>
       </c>
       <c r="S21" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9065840741145468</v>
       </c>
       <c r="T21" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U21" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="V21" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="W21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X21" t="n">
-        <v>0.2145837507256479</v>
+        <v>0.1558640040696549</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.01632925504674202</v>
+        <v>0.01105248000238956</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.01272600575995961</v>
+        <v>0.01270747201495893</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.01390322251207885</v>
+        <v>0.006944174061648009</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.009109279677554262</v>
+        <v>0.009580860541802317</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.01230736222135963</v>
+        <v>0.00647421460009766</v>
       </c>
       <c r="AD21" t="n">
         <v>0</v>
       </c>
       <c r="AE21" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF21" t="n">
         <v>0</v>
       </c>
       <c r="AG21" t="n">
-        <v>0.001314990729519657</v>
+        <v>-0.2022937416699535</v>
       </c>
       <c r="AH21" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="AI21" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="22">
@@ -2638,100 +2638,100 @@
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>9.941107077606285</v>
+        <v>9.932596085307081</v>
       </c>
       <c r="E22" t="n">
-        <v>111.184889376806</v>
+        <v>109.2175520736144</v>
       </c>
       <c r="F22" t="n">
-        <v>2487.570835224308</v>
+        <v>2541.59792883567</v>
       </c>
       <c r="G22" t="n">
-        <v>453167.3359840115</v>
+        <v>449938.2170230591</v>
       </c>
       <c r="H22" t="n">
-        <v>447503.3841271785</v>
+        <v>449798.1704235579</v>
       </c>
       <c r="I22" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="J22" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="K22" t="n">
-        <v>-437.471099866318</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="L22" t="n">
-        <v>0.001314990729519657</v>
+        <v>0</v>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N22" t="n">
         <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>0.2022937416699535</v>
       </c>
       <c r="P22" t="n">
         <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R22" t="n">
-        <v>0.353357323941395</v>
+        <v>0.2022937416699535</v>
       </c>
       <c r="S22" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9065840741145468</v>
       </c>
       <c r="T22" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U22" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="V22" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="W22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X22" t="n">
-        <v>0.2145837507256479</v>
+        <v>0.1558640040696549</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.01632925504674202</v>
+        <v>0.01105248000238956</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.01272600575995961</v>
+        <v>0.01270747201495893</v>
       </c>
       <c r="AA22" t="n">
-        <v>0.01390322251207885</v>
+        <v>0.006944174061648009</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.009109279677554262</v>
+        <v>0.009580860541802317</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.01230736222135963</v>
+        <v>0.00647421460009766</v>
       </c>
       <c r="AD22" t="n">
         <v>0</v>
       </c>
       <c r="AE22" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF22" t="n">
         <v>0</v>
       </c>
       <c r="AG22" t="n">
-        <v>0.001314990729519657</v>
+        <v>-0.2022937416699535</v>
       </c>
       <c r="AH22" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="AI22" t="n">
-        <v>0</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="23">
@@ -2745,100 +2745,100 @@
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>9.941070601379431</v>
+        <v>9.932388190745478</v>
       </c>
       <c r="E23" t="n">
-        <v>111.184889376806</v>
+        <v>109.2175520736144</v>
       </c>
       <c r="F23" t="n">
-        <v>2488.703266143547</v>
+        <v>2541.59792883567</v>
       </c>
       <c r="G23" t="n">
-        <v>453011.0280445975</v>
+        <v>449947.0217928558</v>
       </c>
       <c r="H23" t="n">
-        <v>447503.3841271785</v>
+        <v>449798.1704235579</v>
       </c>
       <c r="I23" t="n">
-        <v>-435.9276050196282</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="J23" t="n">
-        <v>-435.9276050196282</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="K23" t="n">
-        <v>-435.9276050196282</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="L23" t="n">
         <v>0</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N23" t="n">
-        <v>11.89754182370188</v>
+        <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
+        <v>0.204103545786913</v>
       </c>
       <c r="P23" t="n">
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R23" t="n">
-        <v>0.353357323941395</v>
+        <v>0.204103545786913</v>
       </c>
       <c r="S23" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9065840741145468</v>
       </c>
       <c r="T23" t="n">
-        <v>11.89754182370188</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U23" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="V23" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="W23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X23" t="n">
-        <v>0.4822825608341118</v>
+        <v>0.1657660950195598</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.01633320001893058</v>
+        <v>0.01263423942905077</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.01272600575995961</v>
+        <v>0.01270747201495893</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.09248712271356063</v>
+        <v>0.006944174061648009</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.01083107753642307</v>
+        <v>0.01096972840011257</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.01230736222135963</v>
+        <v>0.00647421460009766</v>
       </c>
       <c r="AD23" t="n">
         <v>0</v>
       </c>
       <c r="AE23" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF23" t="n">
         <v>0</v>
       </c>
       <c r="AG23" t="n">
-        <v>0</v>
+        <v>-0.204103545786913</v>
       </c>
       <c r="AH23" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="AI23" t="n">
-        <v>11.89754182370188</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="24">
@@ -2852,100 +2852,100 @@
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>9.941070601379431</v>
+        <v>9.932388190745478</v>
       </c>
       <c r="E24" t="n">
-        <v>111.184889376806</v>
+        <v>109.2175520736144</v>
       </c>
       <c r="F24" t="n">
-        <v>2488.703266143547</v>
+        <v>2541.59792883567</v>
       </c>
       <c r="G24" t="n">
-        <v>453011.0280445975</v>
+        <v>449947.0217928558</v>
       </c>
       <c r="H24" t="n">
-        <v>447503.3841271785</v>
+        <v>449798.1704235579</v>
       </c>
       <c r="I24" t="n">
-        <v>-435.9276050196282</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="J24" t="n">
-        <v>-435.9276050196282</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="K24" t="n">
-        <v>-435.9276050196282</v>
+        <v>-395.6162909681527</v>
       </c>
       <c r="L24" t="n">
         <v>0</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N24" t="n">
-        <v>11.89754182370188</v>
+        <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>0</v>
+        <v>0.204103545786913</v>
       </c>
       <c r="P24" t="n">
         <v>0</v>
       </c>
       <c r="Q24" t="n">
-        <v>0</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="R24" t="n">
-        <v>0.353357323941395</v>
+        <v>0.204103545786913</v>
       </c>
       <c r="S24" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9065840741145468</v>
       </c>
       <c r="T24" t="n">
-        <v>11.89754182370188</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U24" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="V24" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="W24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X24" t="n">
-        <v>0.4822825608341118</v>
+        <v>0.1657660950195598</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.01633320001893058</v>
+        <v>0.01263423942905077</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.01272600575995961</v>
+        <v>0.01270747201495893</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.09248712271356063</v>
+        <v>0.006944174061648009</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.01083107753642307</v>
+        <v>0.01096972840011257</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.01230736222135963</v>
+        <v>0.00647421460009766</v>
       </c>
       <c r="AD24" t="n">
         <v>0</v>
       </c>
       <c r="AE24" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF24" t="n">
         <v>0</v>
       </c>
       <c r="AG24" t="n">
-        <v>0</v>
+        <v>-0.204103545786913</v>
       </c>
       <c r="AH24" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="AI24" t="n">
-        <v>11.89754182370188</v>
+        <v>-24.40625446512856</v>
       </c>
     </row>
     <row r="25">
@@ -2959,40 +2959,40 @@
         <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>9.941070601379431</v>
+        <v>9.932388190745478</v>
       </c>
       <c r="E25" t="n">
-        <v>111.184889376806</v>
+        <v>109.2175520736144</v>
       </c>
       <c r="F25" t="n">
-        <v>2488.511515715455</v>
+        <v>2541.59792883567</v>
       </c>
       <c r="G25" t="n">
-        <v>453621.9804561206</v>
+        <v>449386.734432405</v>
       </c>
       <c r="H25" t="n">
-        <v>446892.412412689</v>
+        <v>449798.1704235579</v>
       </c>
       <c r="I25" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="J25" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="K25" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>0.007612390878211048</v>
       </c>
       <c r="M25" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>0</v>
+        <v>0.204103545786913</v>
       </c>
       <c r="P25" t="n">
         <v>0</v>
@@ -3001,55 +3001,55 @@
         <v>0</v>
       </c>
       <c r="R25" t="n">
-        <v>0.353357323941395</v>
+        <v>0.211715936665124</v>
       </c>
       <c r="S25" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9065840741145468</v>
       </c>
       <c r="T25" t="n">
-        <v>11.89754182370188</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U25" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="V25" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W25" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X25" t="n">
-        <v>0.6113782820154343</v>
+        <v>0.4201050485547848</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.01633320001893058</v>
+        <v>0.0126570766016854</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.01272600575995961</v>
+        <v>0.01270747201495893</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.1281797481846663</v>
+        <v>0.006944174061648009</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.01228010277192983</v>
+        <v>0.08418849179549825</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.01389442786914396</v>
+        <v>0.009534300092644863</v>
       </c>
       <c r="AD25" t="n">
         <v>0</v>
       </c>
       <c r="AE25" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF25" t="n">
         <v>0</v>
       </c>
       <c r="AG25" t="n">
-        <v>0</v>
+        <v>-0.1964911549087019</v>
       </c>
       <c r="AH25" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="AI25" t="n">
         <v>0</v>
@@ -3066,40 +3066,40 @@
         <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>9.941070601379431</v>
+        <v>9.932388190745478</v>
       </c>
       <c r="E26" t="n">
-        <v>111.184889376806</v>
+        <v>109.2175520736144</v>
       </c>
       <c r="F26" t="n">
-        <v>2488.511515715455</v>
+        <v>2541.59792883567</v>
       </c>
       <c r="G26" t="n">
-        <v>453621.9804561206</v>
+        <v>449386.734432405</v>
       </c>
       <c r="H26" t="n">
-        <v>446892.412412689</v>
+        <v>449798.1704235579</v>
       </c>
       <c r="I26" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="J26" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="K26" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="L26" t="n">
-        <v>0</v>
+        <v>0.007612390878211048</v>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
       </c>
       <c r="O26" t="n">
-        <v>0</v>
+        <v>0.204103545786913</v>
       </c>
       <c r="P26" t="n">
         <v>0</v>
@@ -3108,55 +3108,55 @@
         <v>0</v>
       </c>
       <c r="R26" t="n">
-        <v>0.353357323941395</v>
+        <v>0.211715936665124</v>
       </c>
       <c r="S26" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9065840741145468</v>
       </c>
       <c r="T26" t="n">
-        <v>11.89754182370188</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U26" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="V26" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W26" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X26" t="n">
-        <v>0.6113782820154343</v>
+        <v>0.4201050485547848</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.01633320001893058</v>
+        <v>0.0126570766016854</v>
       </c>
       <c r="Z26" t="n">
-        <v>0.01272600575995961</v>
+        <v>0.01270747201495893</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.1281797481846663</v>
+        <v>0.006944174061648009</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.01228010277192983</v>
+        <v>0.08418849179549825</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.01389442786914396</v>
+        <v>0.009534300092644863</v>
       </c>
       <c r="AD26" t="n">
         <v>0</v>
       </c>
       <c r="AE26" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF26" t="n">
         <v>0</v>
       </c>
       <c r="AG26" t="n">
-        <v>0</v>
+        <v>-0.1964911549087019</v>
       </c>
       <c r="AH26" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="AI26" t="n">
         <v>0</v>
@@ -3173,97 +3173,97 @@
         <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>9.941070601379431</v>
+        <v>9.932388190745478</v>
       </c>
       <c r="E27" t="n">
-        <v>111.184889376806</v>
+        <v>109.2346726602747</v>
       </c>
       <c r="F27" t="n">
-        <v>2488.511515715455</v>
+        <v>2541.59792883567</v>
       </c>
       <c r="G27" t="n">
-        <v>453621.9804561206</v>
+        <v>449330.6454754928</v>
       </c>
       <c r="H27" t="n">
-        <v>446892.412412689</v>
+        <v>449798.1704235579</v>
       </c>
       <c r="I27" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="J27" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="K27" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="L27" t="n">
-        <v>0.355191048389313</v>
+        <v>0.007612390878211048</v>
       </c>
       <c r="M27" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N27" t="n">
         <v>0</v>
       </c>
       <c r="O27" t="n">
-        <v>0</v>
+        <v>0.2189689898748548</v>
       </c>
       <c r="P27" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q27" t="n">
         <v>0</v>
       </c>
       <c r="R27" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2265813807530659</v>
       </c>
       <c r="S27" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T27" t="n">
-        <v>11.89754182370188</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U27" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="V27" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="W27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X27" t="n">
-        <v>0.6254489745386255</v>
+        <v>0.4523480016766298</v>
       </c>
       <c r="Y27" t="n">
-        <v>0.01739877316409852</v>
+        <v>0.01580834759698119</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.01272600575995961</v>
+        <v>0.0145272937408192</v>
       </c>
       <c r="AA27" t="n">
-        <v>0.1281797481846663</v>
+        <v>0.0100577270501173</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.01543573738371926</v>
+        <v>0.0857767320224264</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.01389442786914396</v>
+        <v>0.009534300092644863</v>
       </c>
       <c r="AD27" t="n">
         <v>0</v>
       </c>
       <c r="AE27" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF27" t="n">
         <v>0</v>
       </c>
       <c r="AG27" t="n">
-        <v>0.355191048389313</v>
+        <v>-0.2113565989966437</v>
       </c>
       <c r="AH27" t="n">
-        <v>0</v>
+        <v>0.07630269980118909</v>
       </c>
       <c r="AI27" t="n">
         <v>0</v>
@@ -3280,97 +3280,97 @@
         <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>9.941070601379431</v>
+        <v>9.932388190745478</v>
       </c>
       <c r="E28" t="n">
-        <v>111.184889376806</v>
+        <v>109.2346726602747</v>
       </c>
       <c r="F28" t="n">
-        <v>2488.511515715455</v>
+        <v>2541.59792883567</v>
       </c>
       <c r="G28" t="n">
-        <v>453621.9804561206</v>
+        <v>449330.6454754928</v>
       </c>
       <c r="H28" t="n">
-        <v>446892.412412689</v>
+        <v>449798.1704235579</v>
       </c>
       <c r="I28" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="J28" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="K28" t="n">
-        <v>-408.9748149368662</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="L28" t="n">
-        <v>0.355191048389313</v>
+        <v>0.007612390878211048</v>
       </c>
       <c r="M28" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N28" t="n">
         <v>0</v>
       </c>
       <c r="O28" t="n">
-        <v>0</v>
+        <v>0.2189689898748548</v>
       </c>
       <c r="P28" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q28" t="n">
         <v>0</v>
       </c>
       <c r="R28" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2265813807530659</v>
       </c>
       <c r="S28" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T28" t="n">
-        <v>11.89754182370188</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U28" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="V28" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="W28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X28" t="n">
-        <v>0.6254489745386255</v>
+        <v>0.4523480016766298</v>
       </c>
       <c r="Y28" t="n">
-        <v>0.01739877316409852</v>
+        <v>0.01580834759698119</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.01272600575995961</v>
+        <v>0.0145272937408192</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.1281797481846663</v>
+        <v>0.0100577270501173</v>
       </c>
       <c r="AB28" t="n">
-        <v>0.01543573738371926</v>
+        <v>0.0857767320224264</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.01389442786914396</v>
+        <v>0.009534300092644863</v>
       </c>
       <c r="AD28" t="n">
         <v>0</v>
       </c>
       <c r="AE28" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF28" t="n">
         <v>0</v>
       </c>
       <c r="AG28" t="n">
-        <v>0.355191048389313</v>
+        <v>-0.2113565989966437</v>
       </c>
       <c r="AH28" t="n">
-        <v>0</v>
+        <v>0.07630269980118909</v>
       </c>
       <c r="AI28" t="n">
         <v>0</v>
@@ -3387,97 +3387,97 @@
         <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>9.940288908556708</v>
+        <v>9.932388190745478</v>
       </c>
       <c r="E29" t="n">
-        <v>111.184889376806</v>
+        <v>109.2346726602747</v>
       </c>
       <c r="F29" t="n">
-        <v>2491.427533030906</v>
+        <v>2541.695285149893</v>
       </c>
       <c r="G29" t="n">
-        <v>453621.9804561206</v>
+        <v>449330.6454754928</v>
       </c>
       <c r="H29" t="n">
-        <v>446651.587833196</v>
+        <v>449783.917062412</v>
       </c>
       <c r="I29" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="J29" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="K29" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N29" t="n">
         <v>0</v>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
+        <v>0.2189689898748548</v>
       </c>
       <c r="P29" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q29" t="n">
         <v>0</v>
       </c>
       <c r="R29" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2481715594219878</v>
       </c>
       <c r="S29" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T29" t="n">
-        <v>11.89754182370188</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U29" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="V29" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="W29" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X29" t="n">
-        <v>0.6502379675478345</v>
+        <v>0.4633622741021451</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.02004078160575924</v>
+        <v>0.01587311813298796</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.01272600575995961</v>
+        <v>0.0145272937408192</v>
       </c>
       <c r="AA29" t="n">
-        <v>0.1299092656252945</v>
+        <v>0.01167668325763753</v>
       </c>
       <c r="AB29" t="n">
-        <v>0.01543573738371926</v>
+        <v>0.0857767320224264</v>
       </c>
       <c r="AC29" t="n">
-        <v>0.01695959988961769</v>
+        <v>0.01115485507677245</v>
       </c>
       <c r="AD29" t="n">
         <v>0</v>
       </c>
       <c r="AE29" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF29" t="n">
         <v>0</v>
       </c>
       <c r="AG29" t="n">
-        <v>0</v>
+        <v>-0.1897664203277218</v>
       </c>
       <c r="AH29" t="n">
-        <v>0</v>
+        <v>0.07630269980118909</v>
       </c>
       <c r="AI29" t="n">
         <v>0</v>
@@ -3494,97 +3494,97 @@
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>9.940288908556708</v>
+        <v>9.932388190745478</v>
       </c>
       <c r="E30" t="n">
-        <v>111.184889376806</v>
+        <v>109.2346726602747</v>
       </c>
       <c r="F30" t="n">
-        <v>2491.427533030906</v>
+        <v>2541.695285149893</v>
       </c>
       <c r="G30" t="n">
-        <v>453621.9804561206</v>
+        <v>449330.6454754928</v>
       </c>
       <c r="H30" t="n">
-        <v>446651.587833196</v>
+        <v>449783.917062412</v>
       </c>
       <c r="I30" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="J30" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="K30" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="L30" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M30" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N30" t="n">
         <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>0</v>
+        <v>0.2189689898748548</v>
       </c>
       <c r="P30" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
       </c>
       <c r="R30" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2481715594219878</v>
       </c>
       <c r="S30" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T30" t="n">
-        <v>11.89754182370188</v>
+        <v>24.40625446512856</v>
       </c>
       <c r="U30" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="V30" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="W30" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X30" t="n">
-        <v>0.6502379675478345</v>
+        <v>0.4633622741021451</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.02004078160575924</v>
+        <v>0.01587311813298796</v>
       </c>
       <c r="Z30" t="n">
-        <v>0.01272600575995961</v>
+        <v>0.0145272937408192</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.1299092656252945</v>
+        <v>0.01167668325763753</v>
       </c>
       <c r="AB30" t="n">
-        <v>0.01543573738371926</v>
+        <v>0.0857767320224264</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.01695959988961769</v>
+        <v>0.01115485507677245</v>
       </c>
       <c r="AD30" t="n">
         <v>0</v>
       </c>
       <c r="AE30" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF30" t="n">
         <v>0</v>
       </c>
       <c r="AG30" t="n">
-        <v>0</v>
+        <v>-0.1897664203277218</v>
       </c>
       <c r="AH30" t="n">
-        <v>0</v>
+        <v>0.07630269980118909</v>
       </c>
       <c r="AI30" t="n">
         <v>0</v>
@@ -3601,100 +3601,100 @@
         <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>9.940288908556708</v>
+        <v>9.932388190745478</v>
       </c>
       <c r="E31" t="n">
-        <v>111.893628933903</v>
+        <v>109.2074477395399</v>
       </c>
       <c r="F31" t="n">
-        <v>2523.426357140595</v>
+        <v>2541.695285149893</v>
       </c>
       <c r="G31" t="n">
-        <v>446649.3027707326</v>
+        <v>449420.7744118353</v>
       </c>
       <c r="H31" t="n">
-        <v>446651.587833196</v>
+        <v>449783.917062412</v>
       </c>
       <c r="I31" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="J31" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="K31" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M31" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N31" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O31" t="n">
-        <v>0</v>
+        <v>0.2189689898748548</v>
       </c>
       <c r="P31" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q31" t="n">
         <v>0</v>
       </c>
       <c r="R31" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2481715594219878</v>
       </c>
       <c r="S31" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T31" t="n">
-        <v>11.89754182370188</v>
+        <v>83.89867236800386</v>
       </c>
       <c r="U31" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="V31" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="W31" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X31" t="n">
-        <v>0.6833932378009003</v>
+        <v>4.593863068673279</v>
       </c>
       <c r="Y31" t="n">
-        <v>0.02319081646359236</v>
+        <v>0.01902329632814332</v>
       </c>
       <c r="Z31" t="n">
-        <v>0.01443259996571591</v>
+        <v>0.01592184590735177</v>
       </c>
       <c r="AA31" t="n">
-        <v>0.1316798433911429</v>
+        <v>1.244819183197026</v>
       </c>
       <c r="AB31" t="n">
-        <v>0.01875511163020118</v>
+        <v>0.08723974009269038</v>
       </c>
       <c r="AC31" t="n">
-        <v>0.01695959988961769</v>
+        <v>0.01115485507677245</v>
       </c>
       <c r="AD31" t="n">
         <v>0</v>
       </c>
       <c r="AE31" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF31" t="n">
         <v>0</v>
       </c>
       <c r="AG31" t="n">
-        <v>0</v>
+        <v>-0.1897664203277218</v>
       </c>
       <c r="AH31" t="n">
-        <v>0</v>
+        <v>0.07630269980118909</v>
       </c>
       <c r="AI31" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
     </row>
     <row r="32">
@@ -3708,100 +3708,100 @@
         <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>9.940288908556708</v>
+        <v>9.932388190745478</v>
       </c>
       <c r="E32" t="n">
-        <v>111.893628933903</v>
+        <v>109.2074477395399</v>
       </c>
       <c r="F32" t="n">
-        <v>2523.426357140595</v>
+        <v>2541.695285149893</v>
       </c>
       <c r="G32" t="n">
-        <v>446649.3027707326</v>
+        <v>449420.7744118353</v>
       </c>
       <c r="H32" t="n">
-        <v>446651.587833196</v>
+        <v>449783.917062412</v>
       </c>
       <c r="I32" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="J32" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="K32" t="n">
-        <v>-556.3395338430239</v>
+        <v>164.6710694826038</v>
       </c>
       <c r="L32" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M32" t="n">
-        <v>0</v>
+        <v>0.08275832592575103</v>
       </c>
       <c r="N32" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O32" t="n">
-        <v>0</v>
+        <v>0.2189689898748548</v>
       </c>
       <c r="P32" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q32" t="n">
         <v>0</v>
       </c>
       <c r="R32" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2481715594219878</v>
       </c>
       <c r="S32" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T32" t="n">
-        <v>11.89754182370188</v>
+        <v>83.89867236800386</v>
       </c>
       <c r="U32" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="V32" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="W32" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X32" t="n">
-        <v>0.6833932378009003</v>
+        <v>4.593863068673279</v>
       </c>
       <c r="Y32" t="n">
-        <v>0.02319081646359236</v>
+        <v>0.01902329632814332</v>
       </c>
       <c r="Z32" t="n">
-        <v>0.01443259996571591</v>
+        <v>0.01592184590735177</v>
       </c>
       <c r="AA32" t="n">
-        <v>0.1316798433911429</v>
+        <v>1.244819183197026</v>
       </c>
       <c r="AB32" t="n">
-        <v>0.01875511163020118</v>
+        <v>0.08723974009269038</v>
       </c>
       <c r="AC32" t="n">
-        <v>0.01695959988961769</v>
+        <v>0.01115485507677245</v>
       </c>
       <c r="AD32" t="n">
         <v>0</v>
       </c>
       <c r="AE32" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF32" t="n">
         <v>0</v>
       </c>
       <c r="AG32" t="n">
-        <v>0</v>
+        <v>-0.1897664203277218</v>
       </c>
       <c r="AH32" t="n">
-        <v>0</v>
+        <v>0.07630269980118909</v>
       </c>
       <c r="AI32" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
     </row>
     <row r="33">
@@ -3815,100 +3815,100 @@
         <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>9.940288908556708</v>
+        <v>9.931957967666859</v>
       </c>
       <c r="E33" t="n">
-        <v>110.3442699511077</v>
+        <v>109.2016740255957</v>
       </c>
       <c r="F33" t="n">
-        <v>2558.38432262499</v>
+        <v>2541.821094286912</v>
       </c>
       <c r="G33" t="n">
-        <v>445670.9441175979</v>
+        <v>449420.7744118353</v>
       </c>
       <c r="H33" t="n">
-        <v>447628.8838493317</v>
+        <v>449783.917062412</v>
       </c>
       <c r="I33" t="n">
-        <v>-556.3395338430239</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="J33" t="n">
-        <v>-556.3395338430239</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="K33" t="n">
-        <v>-556.3395338430239</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="L33" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M33" t="n">
         <v>0</v>
       </c>
       <c r="N33" t="n">
-        <v>41.16268804653836</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O33" t="n">
-        <v>0</v>
+        <v>0.2189689898748548</v>
       </c>
       <c r="P33" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>0.04526276504436452</v>
       </c>
       <c r="R33" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2481715594219878</v>
       </c>
       <c r="S33" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T33" t="n">
-        <v>53.06022987024024</v>
+        <v>83.94393513304823</v>
       </c>
       <c r="U33" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="V33" t="n">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="W33" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X33" t="n">
-        <v>2.804250460261521</v>
+        <v>4.605395889180572</v>
       </c>
       <c r="Y33" t="n">
-        <v>0.02634089482836341</v>
+        <v>0.02060132689412228</v>
       </c>
       <c r="Z33" t="n">
-        <v>0.01596057745879392</v>
+        <v>0.01617012088512903</v>
       </c>
       <c r="AA33" t="n">
-        <v>0.7601927716234319</v>
+        <v>1.246452723805457</v>
       </c>
       <c r="AB33" t="n">
-        <v>0.02033354973995329</v>
+        <v>0.08723974009269038</v>
       </c>
       <c r="AC33" t="n">
-        <v>0.01844734442791375</v>
+        <v>0.01115485507677245</v>
       </c>
       <c r="AD33" t="n">
         <v>0</v>
       </c>
       <c r="AE33" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF33" t="n">
         <v>0</v>
       </c>
       <c r="AG33" t="n">
-        <v>0</v>
+        <v>-0.1897664203277218</v>
       </c>
       <c r="AH33" t="n">
-        <v>0</v>
+        <v>-0.006455626124561932</v>
       </c>
       <c r="AI33" t="n">
-        <v>41.16268804653836</v>
+        <v>59.44715513783093</v>
       </c>
     </row>
     <row r="34">
@@ -3922,100 +3922,100 @@
         <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>9.940288908556708</v>
+        <v>9.931957967666859</v>
       </c>
       <c r="E34" t="n">
-        <v>110.3442699511077</v>
+        <v>109.2016740255957</v>
       </c>
       <c r="F34" t="n">
-        <v>2558.38432262499</v>
+        <v>2541.821094286912</v>
       </c>
       <c r="G34" t="n">
-        <v>445670.9441175979</v>
+        <v>449420.7744118353</v>
       </c>
       <c r="H34" t="n">
-        <v>447628.8838493317</v>
+        <v>449783.917062412</v>
       </c>
       <c r="I34" t="n">
-        <v>-556.3395338430239</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="J34" t="n">
-        <v>-556.3395338430239</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="K34" t="n">
-        <v>-556.3395338430239</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M34" t="n">
         <v>0</v>
       </c>
       <c r="N34" t="n">
-        <v>41.16268804653836</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O34" t="n">
-        <v>0</v>
+        <v>0.2189689898748548</v>
       </c>
       <c r="P34" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q34" t="n">
-        <v>0</v>
+        <v>0.04526276504436452</v>
       </c>
       <c r="R34" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2481715594219878</v>
       </c>
       <c r="S34" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T34" t="n">
-        <v>53.06022987024024</v>
+        <v>83.94393513304823</v>
       </c>
       <c r="U34" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="V34" t="n">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="W34" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X34" t="n">
-        <v>2.804250460261521</v>
+        <v>4.605395889180572</v>
       </c>
       <c r="Y34" t="n">
-        <v>0.02634089482836341</v>
+        <v>0.02060132689412228</v>
       </c>
       <c r="Z34" t="n">
-        <v>0.01596057745879392</v>
+        <v>0.01617012088512903</v>
       </c>
       <c r="AA34" t="n">
-        <v>0.7601927716234319</v>
+        <v>1.246452723805457</v>
       </c>
       <c r="AB34" t="n">
-        <v>0.02033354973995329</v>
+        <v>0.08723974009269038</v>
       </c>
       <c r="AC34" t="n">
-        <v>0.01844734442791375</v>
+        <v>0.01115485507677245</v>
       </c>
       <c r="AD34" t="n">
         <v>0</v>
       </c>
       <c r="AE34" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF34" t="n">
         <v>0</v>
       </c>
       <c r="AG34" t="n">
-        <v>0</v>
+        <v>-0.1897664203277218</v>
       </c>
       <c r="AH34" t="n">
-        <v>0</v>
+        <v>-0.006455626124561932</v>
       </c>
       <c r="AI34" t="n">
-        <v>41.16268804653836</v>
+        <v>59.44715513783093</v>
       </c>
     </row>
     <row r="35">
@@ -4029,100 +4029,100 @@
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>9.940288908556708</v>
+        <v>9.931957967666859</v>
       </c>
       <c r="E35" t="n">
-        <v>110.3442699511077</v>
+        <v>109.2016740255957</v>
       </c>
       <c r="F35" t="n">
-        <v>2548.270665467356</v>
+        <v>2541.821094286912</v>
       </c>
       <c r="G35" t="n">
-        <v>445670.9441175979</v>
+        <v>449420.7744118353</v>
       </c>
       <c r="H35" t="n">
-        <v>449263.9736295015</v>
+        <v>449783.917062412</v>
       </c>
       <c r="I35" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="J35" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="K35" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="L35" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M35" t="n">
         <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O35" t="n">
-        <v>0</v>
+        <v>0.2218186181169236</v>
       </c>
       <c r="P35" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q35" t="n">
-        <v>0</v>
+        <v>0.04526276504436452</v>
       </c>
       <c r="R35" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2510211876640567</v>
       </c>
       <c r="S35" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T35" t="n">
-        <v>53.06022987024024</v>
+        <v>83.94393513304823</v>
       </c>
       <c r="U35" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="V35" t="n">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="W35" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="X35" t="n">
-        <v>3.236234225061722</v>
+        <v>4.615896438618727</v>
       </c>
       <c r="Y35" t="n">
-        <v>0.02949095386140562</v>
+        <v>0.02375149172556893</v>
       </c>
       <c r="Z35" t="n">
-        <v>0.01596057745879392</v>
+        <v>0.01617012088512903</v>
       </c>
       <c r="AA35" t="n">
-        <v>0.8851823938953498</v>
+        <v>1.246452723805457</v>
       </c>
       <c r="AB35" t="n">
-        <v>0.02033354973995329</v>
+        <v>0.08723974009269038</v>
       </c>
       <c r="AC35" t="n">
-        <v>0.01990279256301412</v>
+        <v>0.01115485507677245</v>
       </c>
       <c r="AD35" t="n">
         <v>0</v>
       </c>
       <c r="AE35" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF35" t="n">
         <v>0</v>
       </c>
       <c r="AG35" t="n">
-        <v>0</v>
+        <v>-0.1926160485697906</v>
       </c>
       <c r="AH35" t="n">
-        <v>0</v>
+        <v>-0.006455626124561932</v>
       </c>
       <c r="AI35" t="n">
-        <v>0</v>
+        <v>59.44715513783093</v>
       </c>
     </row>
     <row r="36">
@@ -4136,100 +4136,100 @@
         <v>1</v>
       </c>
       <c r="D36" t="n">
-        <v>9.940288908556708</v>
+        <v>9.931957967666859</v>
       </c>
       <c r="E36" t="n">
-        <v>110.3442699511077</v>
+        <v>109.2016740255957</v>
       </c>
       <c r="F36" t="n">
-        <v>2548.270665467356</v>
+        <v>2541.821094286912</v>
       </c>
       <c r="G36" t="n">
-        <v>445670.9441175979</v>
+        <v>449420.7744118353</v>
       </c>
       <c r="H36" t="n">
-        <v>449263.9736295015</v>
+        <v>449783.917062412</v>
       </c>
       <c r="I36" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="J36" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="K36" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M36" t="n">
         <v>0</v>
       </c>
       <c r="N36" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O36" t="n">
-        <v>0</v>
+        <v>0.2218186181169236</v>
       </c>
       <c r="P36" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q36" t="n">
-        <v>0</v>
+        <v>0.04526276504436452</v>
       </c>
       <c r="R36" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2510211876640567</v>
       </c>
       <c r="S36" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T36" t="n">
-        <v>53.06022987024024</v>
+        <v>83.94393513304823</v>
       </c>
       <c r="U36" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="V36" t="n">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="W36" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="X36" t="n">
-        <v>3.236234225061722</v>
+        <v>4.615896438618727</v>
       </c>
       <c r="Y36" t="n">
-        <v>0.02949095386140562</v>
+        <v>0.02375149172556893</v>
       </c>
       <c r="Z36" t="n">
-        <v>0.01596057745879392</v>
+        <v>0.01617012088512903</v>
       </c>
       <c r="AA36" t="n">
-        <v>0.8851823938953498</v>
+        <v>1.246452723805457</v>
       </c>
       <c r="AB36" t="n">
-        <v>0.02033354973995329</v>
+        <v>0.08723974009269038</v>
       </c>
       <c r="AC36" t="n">
-        <v>0.01990279256301412</v>
+        <v>0.01115485507677245</v>
       </c>
       <c r="AD36" t="n">
         <v>0</v>
       </c>
       <c r="AE36" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF36" t="n">
         <v>0</v>
       </c>
       <c r="AG36" t="n">
-        <v>0</v>
+        <v>-0.1926160485697906</v>
       </c>
       <c r="AH36" t="n">
-        <v>0</v>
+        <v>-0.006455626124561932</v>
       </c>
       <c r="AI36" t="n">
-        <v>0</v>
+        <v>59.44715513783093</v>
       </c>
     </row>
     <row r="37">
@@ -4243,100 +4243,100 @@
         <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>9.940288908556708</v>
+        <v>9.932066785138028</v>
       </c>
       <c r="E37" t="n">
-        <v>110.3442699511077</v>
+        <v>109.2016740255957</v>
       </c>
       <c r="F37" t="n">
-        <v>2548.270665467356</v>
+        <v>2541.821094286912</v>
       </c>
       <c r="G37" t="n">
-        <v>445670.9441175979</v>
+        <v>449420.7744118353</v>
       </c>
       <c r="H37" t="n">
-        <v>449263.9736295015</v>
+        <v>449779.3104759637</v>
       </c>
       <c r="I37" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="J37" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="K37" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M37" t="n">
         <v>0</v>
       </c>
       <c r="N37" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O37" t="n">
-        <v>0</v>
+        <v>0.2218186181169236</v>
       </c>
       <c r="P37" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q37" t="n">
-        <v>0</v>
+        <v>0.04526276504436452</v>
       </c>
       <c r="R37" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2510211876640567</v>
       </c>
       <c r="S37" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T37" t="n">
-        <v>53.06022987024024</v>
+        <v>83.94393513304823</v>
       </c>
       <c r="U37" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="V37" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="W37" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="X37" t="n">
-        <v>3.246469136345045</v>
+        <v>4.626636080788884</v>
       </c>
       <c r="Y37" t="n">
-        <v>0.02949095386140562</v>
+        <v>0.02532207840258646</v>
       </c>
       <c r="Z37" t="n">
-        <v>0.01596057745879392</v>
+        <v>0.01617012088512903</v>
       </c>
       <c r="AA37" t="n">
-        <v>0.8851823938953498</v>
+        <v>1.246452723805457</v>
       </c>
       <c r="AB37" t="n">
-        <v>0.02033354973995329</v>
+        <v>0.08723974009269038</v>
       </c>
       <c r="AC37" t="n">
-        <v>0.02297326594801106</v>
+        <v>0.01280616105080183</v>
       </c>
       <c r="AD37" t="n">
         <v>0</v>
       </c>
       <c r="AE37" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF37" t="n">
         <v>0</v>
       </c>
       <c r="AG37" t="n">
-        <v>0</v>
+        <v>-0.1926160485697906</v>
       </c>
       <c r="AH37" t="n">
-        <v>0</v>
+        <v>-0.006455626124561932</v>
       </c>
       <c r="AI37" t="n">
-        <v>0</v>
+        <v>59.44715513783093</v>
       </c>
     </row>
     <row r="38">
@@ -4350,100 +4350,100 @@
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>9.940288908556708</v>
+        <v>9.932066785138028</v>
       </c>
       <c r="E38" t="n">
-        <v>110.3442699511077</v>
+        <v>109.2016740255957</v>
       </c>
       <c r="F38" t="n">
-        <v>2548.270665467356</v>
+        <v>2541.821094286912</v>
       </c>
       <c r="G38" t="n">
-        <v>445670.9441175979</v>
+        <v>449420.7744118353</v>
       </c>
       <c r="H38" t="n">
-        <v>449263.9736295015</v>
+        <v>449779.3104759637</v>
       </c>
       <c r="I38" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="J38" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="K38" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="L38" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M38" t="n">
         <v>0</v>
       </c>
       <c r="N38" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O38" t="n">
-        <v>0</v>
+        <v>0.2218186181169236</v>
       </c>
       <c r="P38" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q38" t="n">
-        <v>0</v>
+        <v>0.04526276504436452</v>
       </c>
       <c r="R38" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2510211876640567</v>
       </c>
       <c r="S38" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T38" t="n">
-        <v>53.06022987024024</v>
+        <v>83.94393513304823</v>
       </c>
       <c r="U38" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="V38" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="W38" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="X38" t="n">
-        <v>3.246469136345045</v>
+        <v>4.626636080788884</v>
       </c>
       <c r="Y38" t="n">
-        <v>0.02949095386140562</v>
+        <v>0.02532207840258646</v>
       </c>
       <c r="Z38" t="n">
-        <v>0.01596057745879392</v>
+        <v>0.01617012088512903</v>
       </c>
       <c r="AA38" t="n">
-        <v>0.8851823938953498</v>
+        <v>1.246452723805457</v>
       </c>
       <c r="AB38" t="n">
-        <v>0.02033354973995329</v>
+        <v>0.08723974009269038</v>
       </c>
       <c r="AC38" t="n">
-        <v>0.02297326594801106</v>
+        <v>0.01280616105080183</v>
       </c>
       <c r="AD38" t="n">
         <v>0</v>
       </c>
       <c r="AE38" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF38" t="n">
         <v>0</v>
       </c>
       <c r="AG38" t="n">
-        <v>0</v>
+        <v>-0.1926160485697906</v>
       </c>
       <c r="AH38" t="n">
-        <v>0</v>
+        <v>-0.006455626124561932</v>
       </c>
       <c r="AI38" t="n">
-        <v>0</v>
+        <v>59.44715513783093</v>
       </c>
     </row>
     <row r="39">
@@ -4457,100 +4457,100 @@
         <v>1</v>
       </c>
       <c r="D39" t="n">
-        <v>9.944849962994249</v>
+        <v>9.932066785138028</v>
       </c>
       <c r="E39" t="n">
-        <v>110.2829699509824</v>
+        <v>109.2016740255957</v>
       </c>
       <c r="F39" t="n">
-        <v>2548.902006282849</v>
+        <v>2535.987289686373</v>
       </c>
       <c r="G39" t="n">
-        <v>445584.6789642543</v>
+        <v>450215.1535063742</v>
       </c>
       <c r="H39" t="n">
-        <v>449263.9736295015</v>
+        <v>449779.3104759637</v>
       </c>
       <c r="I39" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="J39" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="K39" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="L39" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M39" t="n">
         <v>0</v>
       </c>
       <c r="N39" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O39" t="n">
-        <v>0</v>
+        <v>0.2218186181169236</v>
       </c>
       <c r="P39" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q39" t="n">
-        <v>0</v>
+        <v>0.1876553677220388</v>
       </c>
       <c r="R39" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2510211876640567</v>
       </c>
       <c r="S39" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T39" t="n">
-        <v>53.06022987024024</v>
+        <v>84.0863277357259</v>
       </c>
       <c r="U39" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="V39" t="n">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="W39" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="X39" t="n">
-        <v>3.26739242153511</v>
+        <v>4.646063654522647</v>
       </c>
       <c r="Y39" t="n">
-        <v>0.0310624902304367</v>
+        <v>0.02532207840258646</v>
       </c>
       <c r="Z39" t="n">
-        <v>0.01723749808019774</v>
+        <v>0.01932054319225331</v>
       </c>
       <c r="AA39" t="n">
-        <v>0.8869297333330971</v>
+        <v>1.247775649221221</v>
       </c>
       <c r="AB39" t="n">
-        <v>0.02201473886879038</v>
+        <v>0.08859466448993168</v>
       </c>
       <c r="AC39" t="n">
-        <v>0.02297326594801106</v>
+        <v>0.01280616105080183</v>
       </c>
       <c r="AD39" t="n">
         <v>0</v>
       </c>
       <c r="AE39" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF39" t="n">
         <v>0</v>
       </c>
       <c r="AG39" t="n">
-        <v>0</v>
+        <v>-0.1926160485697906</v>
       </c>
       <c r="AH39" t="n">
-        <v>0</v>
+        <v>-0.006455626124561932</v>
       </c>
       <c r="AI39" t="n">
-        <v>0</v>
+        <v>59.30476253515326</v>
       </c>
     </row>
     <row r="40">
@@ -4564,100 +4564,100 @@
         <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>9.944849962994249</v>
+        <v>9.932066785138028</v>
       </c>
       <c r="E40" t="n">
-        <v>110.2829699509824</v>
+        <v>109.2016740255957</v>
       </c>
       <c r="F40" t="n">
-        <v>2548.902006282849</v>
+        <v>2535.987289686373</v>
       </c>
       <c r="G40" t="n">
-        <v>445584.6789642543</v>
+        <v>450215.1535063742</v>
       </c>
       <c r="H40" t="n">
-        <v>449263.9736295015</v>
+        <v>449779.3104759637</v>
       </c>
       <c r="I40" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="J40" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="K40" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="L40" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M40" t="n">
         <v>0</v>
       </c>
       <c r="N40" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O40" t="n">
-        <v>0</v>
+        <v>0.2218186181169236</v>
       </c>
       <c r="P40" t="n">
-        <v>0</v>
+        <v>0.006455626124561932</v>
       </c>
       <c r="Q40" t="n">
-        <v>0</v>
+        <v>0.1876553677220388</v>
       </c>
       <c r="R40" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2510211876640567</v>
       </c>
       <c r="S40" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9130397002391087</v>
       </c>
       <c r="T40" t="n">
-        <v>53.06022987024024</v>
+        <v>84.0863277357259</v>
       </c>
       <c r="U40" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="V40" t="n">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="W40" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="X40" t="n">
-        <v>3.26739242153511</v>
+        <v>4.646063654522647</v>
       </c>
       <c r="Y40" t="n">
-        <v>0.0310624902304367</v>
+        <v>0.02532207840258646</v>
       </c>
       <c r="Z40" t="n">
-        <v>0.01723749808019774</v>
+        <v>0.01932054319225331</v>
       </c>
       <c r="AA40" t="n">
-        <v>0.8869297333330971</v>
+        <v>1.247775649221221</v>
       </c>
       <c r="AB40" t="n">
-        <v>0.02201473886879038</v>
+        <v>0.08859466448993168</v>
       </c>
       <c r="AC40" t="n">
-        <v>0.02297326594801106</v>
+        <v>0.01280616105080183</v>
       </c>
       <c r="AD40" t="n">
         <v>0</v>
       </c>
       <c r="AE40" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF40" t="n">
         <v>0</v>
       </c>
       <c r="AG40" t="n">
-        <v>0</v>
+        <v>-0.1926160485697906</v>
       </c>
       <c r="AH40" t="n">
-        <v>0</v>
+        <v>-0.006455626124561932</v>
       </c>
       <c r="AI40" t="n">
-        <v>0</v>
+        <v>59.30476253515326</v>
       </c>
     </row>
     <row r="41">
@@ -4671,100 +4671,100 @@
         <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>9.944849962994249</v>
+        <v>9.931066122855443</v>
       </c>
       <c r="E41" t="n">
-        <v>110.2829699509824</v>
+        <v>109.2128448101583</v>
       </c>
       <c r="F41" t="n">
-        <v>2548.902006282849</v>
+        <v>2535.987289686373</v>
       </c>
       <c r="G41" t="n">
-        <v>445799.7810061803</v>
+        <v>450221.0739956938</v>
       </c>
       <c r="H41" t="n">
-        <v>449048.838965239</v>
+        <v>449779.1238194008</v>
       </c>
       <c r="I41" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="J41" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="K41" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M41" t="n">
         <v>0</v>
       </c>
       <c r="N41" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O41" t="n">
-        <v>0</v>
+        <v>0.2218186181169236</v>
       </c>
       <c r="P41" t="n">
-        <v>0</v>
+        <v>0.008144068771714582</v>
       </c>
       <c r="Q41" t="n">
-        <v>0</v>
+        <v>0.1876553677220388</v>
       </c>
       <c r="R41" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2510211876640567</v>
       </c>
       <c r="S41" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9147281428862614</v>
       </c>
       <c r="T41" t="n">
-        <v>53.06022987024024</v>
+        <v>84.0863277357259</v>
       </c>
       <c r="U41" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="V41" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="W41" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="X41" t="n">
-        <v>3.277704491913036</v>
+        <v>4.677447087514342</v>
       </c>
       <c r="Y41" t="n">
-        <v>0.0310624902304367</v>
+        <v>0.0269048454502881</v>
       </c>
       <c r="Z41" t="n">
-        <v>0.01723749808019774</v>
+        <v>0.0210347273254011</v>
       </c>
       <c r="AA41" t="n">
-        <v>0.8869297333330971</v>
+        <v>1.247775649221221</v>
       </c>
       <c r="AB41" t="n">
-        <v>0.02343996624061243</v>
+        <v>0.09298269197141902</v>
       </c>
       <c r="AC41" t="n">
-        <v>0.02464165968956681</v>
+        <v>0.01453621228597342</v>
       </c>
       <c r="AD41" t="n">
         <v>0</v>
       </c>
       <c r="AE41" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF41" t="n">
         <v>0</v>
       </c>
       <c r="AG41" t="n">
-        <v>0</v>
+        <v>-0.1926160485697906</v>
       </c>
       <c r="AH41" t="n">
-        <v>0</v>
+        <v>-0.008144068771714582</v>
       </c>
       <c r="AI41" t="n">
-        <v>0</v>
+        <v>59.30476253515326</v>
       </c>
     </row>
     <row r="42">
@@ -4778,100 +4778,100 @@
         <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>9.944849962994249</v>
+        <v>9.931066122855443</v>
       </c>
       <c r="E42" t="n">
-        <v>110.2829699509824</v>
+        <v>109.2128448101583</v>
       </c>
       <c r="F42" t="n">
-        <v>2548.902006282849</v>
+        <v>2535.987289686373</v>
       </c>
       <c r="G42" t="n">
-        <v>445799.7810061803</v>
+        <v>450221.0739956938</v>
       </c>
       <c r="H42" t="n">
-        <v>449048.838965239</v>
+        <v>449779.1238194008</v>
       </c>
       <c r="I42" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="J42" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="K42" t="n">
-        <v>-705.7224107523067</v>
+        <v>183.9287139812832</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>0.02920256954713303</v>
       </c>
       <c r="M42" t="n">
         <v>0</v>
       </c>
       <c r="N42" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O42" t="n">
-        <v>0</v>
+        <v>0.2218186181169236</v>
       </c>
       <c r="P42" t="n">
-        <v>0</v>
+        <v>0.008144068771714582</v>
       </c>
       <c r="Q42" t="n">
-        <v>0</v>
+        <v>0.1876553677220388</v>
       </c>
       <c r="R42" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2510211876640567</v>
       </c>
       <c r="S42" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9147281428862614</v>
       </c>
       <c r="T42" t="n">
-        <v>53.06022987024024</v>
+        <v>84.0863277357259</v>
       </c>
       <c r="U42" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="V42" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="W42" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="X42" t="n">
-        <v>3.277704491913036</v>
+        <v>4.677447087514342</v>
       </c>
       <c r="Y42" t="n">
-        <v>0.0310624902304367</v>
+        <v>0.0269048454502881</v>
       </c>
       <c r="Z42" t="n">
-        <v>0.01723749808019774</v>
+        <v>0.0210347273254011</v>
       </c>
       <c r="AA42" t="n">
-        <v>0.8869297333330971</v>
+        <v>1.247775649221221</v>
       </c>
       <c r="AB42" t="n">
-        <v>0.02343996624061243</v>
+        <v>0.09298269197141902</v>
       </c>
       <c r="AC42" t="n">
-        <v>0.02464165968956681</v>
+        <v>0.01453621228597342</v>
       </c>
       <c r="AD42" t="n">
         <v>0</v>
       </c>
       <c r="AE42" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF42" t="n">
         <v>0</v>
       </c>
       <c r="AG42" t="n">
-        <v>0</v>
+        <v>-0.1926160485697906</v>
       </c>
       <c r="AH42" t="n">
-        <v>0</v>
+        <v>-0.008144068771714582</v>
       </c>
       <c r="AI42" t="n">
-        <v>0</v>
+        <v>59.30476253515326</v>
       </c>
     </row>
     <row r="43">
@@ -4885,28 +4885,28 @@
         <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>9.944849962994249</v>
+        <v>9.933046870866811</v>
       </c>
       <c r="E43" t="n">
-        <v>110.2829699509824</v>
+        <v>109.2375335622838</v>
       </c>
       <c r="F43" t="n">
-        <v>2537.701370873694</v>
+        <v>2535.987289686373</v>
       </c>
       <c r="G43" t="n">
-        <v>445799.7810061803</v>
+        <v>450154.5863575673</v>
       </c>
       <c r="H43" t="n">
-        <v>450325.6052309144</v>
+        <v>449779.1238194008</v>
       </c>
       <c r="I43" t="n">
-        <v>-705.7224107523067</v>
+        <v>105.4341854007644</v>
       </c>
       <c r="J43" t="n">
-        <v>-705.7224107523067</v>
+        <v>105.4341854007644</v>
       </c>
       <c r="K43" t="n">
-        <v>-705.7224107523067</v>
+        <v>105.4341854007644</v>
       </c>
       <c r="L43" t="n">
         <v>0</v>
@@ -4915,70 +4915,70 @@
         <v>0</v>
       </c>
       <c r="N43" t="n">
-        <v>0</v>
+        <v>59.4924179028753</v>
       </c>
       <c r="O43" t="n">
-        <v>0</v>
+        <v>0.2218186181169236</v>
       </c>
       <c r="P43" t="n">
-        <v>0</v>
+        <v>0.008144068771714582</v>
       </c>
       <c r="Q43" t="n">
-        <v>0</v>
+        <v>0.1876553677220388</v>
       </c>
       <c r="R43" t="n">
-        <v>0.708548372330708</v>
+        <v>0.2510211876640567</v>
       </c>
       <c r="S43" t="n">
-        <v>0.08523664219493264</v>
+        <v>0.9147281428862614</v>
       </c>
       <c r="T43" t="n">
-        <v>53.06022987024024</v>
+        <v>84.0863277357259</v>
       </c>
       <c r="U43" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="V43" t="n">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="W43" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="X43" t="n">
-        <v>3.29356737848561</v>
+        <v>4.693869623294643</v>
       </c>
       <c r="Y43" t="n">
-        <v>0.0310624902304367</v>
+        <v>0.0269924531589295</v>
       </c>
       <c r="Z43" t="n">
-        <v>0.01723749808019774</v>
+        <v>0.02360473077419016</v>
       </c>
       <c r="AA43" t="n">
-        <v>0.8907764964405515</v>
+        <v>1.247775649221221</v>
       </c>
       <c r="AB43" t="n">
-        <v>0.02343996624061243</v>
+        <v>0.09525184154807874</v>
       </c>
       <c r="AC43" t="n">
-        <v>0.02555376255388501</v>
+        <v>0.01453621228597342</v>
       </c>
       <c r="AD43" t="n">
         <v>0</v>
       </c>
       <c r="AE43" t="n">
-        <v>0</v>
+        <v>-24.80589667011246</v>
       </c>
       <c r="AF43" t="n">
         <v>0</v>
       </c>
       <c r="AG43" t="n">
-        <v>0</v>
+        <v>-0.2218186181169236</v>
       </c>
       <c r="AH43" t="n">
-        <v>0</v>
+        <v>-0.008144068771714582</v>
       </c>
       <c r="AI43" t="n">
-        <v>0</v>
+        <v>59.30476253515326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>